<commit_message>
commit before branch to work on new additions
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_ip_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_ip_calibrated.xlsx
@@ -15283,112 +15283,112 @@
         <v>0.8</v>
       </c>
       <c r="J114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="K114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="L114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="M114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="N114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="O114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="P114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="Q114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="R114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="S114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="T114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="U114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="V114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="W114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="X114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="Y114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="Z114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AA114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AB114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AC114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AD114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AE114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AF114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AG114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AH114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AI114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AJ114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AK114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AL114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AM114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AN114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AO114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AP114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AQ114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AR114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
       <c r="AS114" t="n">
-        <v>622448667.1</v>
+        <v>16463.89538</v>
       </c>
     </row>
     <row r="115">

</xml_diff>